<commit_message>
Mark latrine questions as required
</commit_message>
<xml_diff>
--- a/odkx/app/config/tables/hh_latrine/forms/hh_latrine/hh_latrine.xlsx
+++ b/odkx/app/config/tables/hh_latrine/forms/hh_latrine/hh_latrine.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="112">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t xml:space="preserve">inputAttributes.step</t>
+  </si>
+  <si>
+    <t xml:space="preserve">required</t>
   </si>
   <si>
     <t xml:space="preserve">begin screen</t>
@@ -550,7 +553,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.64453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.65625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="8.69"/>
   </cols>
@@ -1589,13 +1592,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.23828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.03"/>
@@ -1636,73 +1639,82 @@
       <c r="I1" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="J1" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H8" s="0" t="n">
         <v>1</v>
@@ -1710,10 +1722,13 @@
       <c r="I8" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="J8" s="0" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1738,7 +1753,7 @@
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.23828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="23.75"/>
@@ -1746,112 +1761,112 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1872,11 +1887,11 @@
   </sheetPr>
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.64453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.65625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.33"/>
@@ -1891,71 +1906,71 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>20210304001</v>
+        <v>20210421001</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
@@ -1963,49 +1978,49 @@
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>1</v>
@@ -3023,7 +3038,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.64453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.65625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.14"/>
@@ -3043,42 +3058,42 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -4097,7 +4112,7 @@
       <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.26171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="37.56"/>
@@ -4105,198 +4120,198 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>68</v>
-      </c>
       <c r="C1" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update PT translation for latrines
April requests row 39
</commit_message>
<xml_diff>
--- a/odkx/app/config/tables/hh_latrine/forms/hh_latrine/hh_latrine.xlsx
+++ b/odkx/app/config/tables/hh_latrine/forms/hh_latrine/hh_latrine.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" state="visible" r:id="rId2"/>
@@ -321,7 +321,7 @@
     <t xml:space="preserve">Latrine with unventilated slab</t>
   </si>
   <si>
-    <t xml:space="preserve">Latrina com laje ventilada</t>
+    <t xml:space="preserve">Latrina com laje não ventilada</t>
   </si>
   <si>
     <t xml:space="preserve">Choo cha shimo kisichokuwa na bomba la hewa</t>
@@ -443,13 +443,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -553,9 +557,9 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.65625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.8671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="8.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="8.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1579,7 +1583,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1598,17 +1602,17 @@
       <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.23828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="34.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="32.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1734,7 +1738,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1753,10 +1757,10 @@
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.23828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="23.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="22.47"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1872,7 +1876,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1887,21 +1891,21 @@
   </sheetPr>
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.65625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.8671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="9" style="0" width="8.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="9" style="0" width="8.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3019,7 +3023,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3038,11 +3042,11 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.65625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.8671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="0" width="8.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="0" width="8.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4093,7 +4097,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4108,14 +4112,14 @@
   </sheetPr>
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.26171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.65625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="37.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="35.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4244,14 +4248,14 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>42</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="2" t="s">
         <v>98</v>
       </c>
       <c r="D10" s="0" t="s">
@@ -4315,14 +4319,14 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:D4 B6:D1048576 B5">
+  <conditionalFormatting sqref="B1:D4 B6:D9 B5 B11:D1048576 B10 D10">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>